<commit_message>
add dictionary examples excel
</commit_message>
<xml_diff>
--- a/Examples/Dictionary/Calc/Exp104_RatingsSetup_empty.xlsx
+++ b/Examples/Dictionary/Calc/Exp104_RatingsSetup_empty.xlsx
@@ -1263,7 +1263,61 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="36">
+  <dataValidations count="54">
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A19:A21</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A19:A21</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A19:A21</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A19:A21</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A19:A21</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A19:A21</formula1>
+    </dataValidation>
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=rating_scales!A3:A5</formula1>
     </dataValidation>

</xml_diff>